<commit_message>
Added LavaWrap to materials and modified plotting slightly. I need to adjust how plotting is done so it's not just a bunch of commented out lines, but for now that's what it is. I had a weird problem with reading materials from excel. I had to specify to read from columsn C:ZZ because I couldn't just say "read until you have read all the materials". I'll have to fix that in the future
</commit_message>
<xml_diff>
--- a/Material_Properties.xlsx
+++ b/Material_Properties.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Transfer\Fraser Jones\1D Transient Toolbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Transfer\Fraser Jones\1D_Transient_Toolbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA67D92-1418-4CE4-8538-F4C166E24D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B12C9B-76E5-4BC5-B3D5-792BAE9C2BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" xr2:uid="{5FC984CA-FA47-49C6-B571-C8119F27FD36}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5FC984CA-FA47-49C6-B571-C8119F27FD36}"/>
   </bookViews>
   <sheets>
     <sheet name="Material Properties" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
   <si>
     <t>Material</t>
   </si>
@@ -290,6 +290,9 @@
   </si>
   <si>
     <t>Cryogel</t>
+  </si>
+  <si>
+    <t>LavaWrap</t>
   </si>
 </sst>
 </file>
@@ -329,7 +332,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -352,11 +355,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -379,12 +393,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -392,6 +400,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -845,10 +862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{476E0231-AF0F-4564-A165-BC653E59D282}">
-  <dimension ref="A1:X35"/>
+  <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,9 +873,10 @@
     <col min="1" max="1" width="81.42578125" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -924,15 +942,18 @@
       <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="X1" s="8" t="s">
         <v>68</v>
       </c>
+      <c r="Y1" s="8" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -998,35 +1019,38 @@
       <c r="W2" s="2">
         <v>0.3</v>
       </c>
-      <c r="X2" s="12">
+      <c r="X2" s="10">
         <v>1.1037E-2</v>
       </c>
+      <c r="Y2" s="2">
+        <v>3.5000000000000003E-2</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="9">
         <v>-2.22E-4</v>
       </c>
       <c r="E3" s="3">
         <v>0</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="9">
         <v>7.5099999999999996E-5</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="9">
         <v>1.09E-2</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="9">
         <v>1.09E-2</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="9">
         <v>1.09E-2</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="9">
         <v>1.3900000000000001E-5</v>
       </c>
       <c r="K3" s="3">
@@ -1068,17 +1092,20 @@
       <c r="W3" s="3">
         <v>0</v>
       </c>
-      <c r="X3" s="11">
+      <c r="X3" s="9">
         <v>2.0000000000000002E-5</v>
       </c>
+      <c r="Y3" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <v>4.82E-7</v>
       </c>
       <c r="E4" s="3">
@@ -1087,13 +1114,13 @@
       <c r="F4" s="3">
         <v>0</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="9">
         <v>-4.6400000000000003E-5</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="9">
         <v>-4.6400000000000003E-5</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="9">
         <v>-4.6400000000000003E-5</v>
       </c>
       <c r="J4" s="3">
@@ -1141,14 +1168,17 @@
       <c r="X4" s="3">
         <v>0</v>
       </c>
+      <c r="Y4" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="9">
         <v>-2.1E-10</v>
       </c>
       <c r="E5" s="3">
@@ -1157,13 +1187,13 @@
       <c r="F5" s="3">
         <v>0</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="9">
         <v>8.6000000000000002E-8</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <v>8.6000000000000002E-8</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="9">
         <v>8.6000000000000002E-8</v>
       </c>
       <c r="J5" s="3">
@@ -1211,10 +1241,13 @@
       <c r="X5" s="3">
         <v>0</v>
       </c>
+      <c r="Y5" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="1" t="s">
         <v>27</v>
       </c>
@@ -1227,13 +1260,13 @@
       <c r="F6" s="3">
         <v>0</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="9">
         <v>-5.8599999999999997E-11</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <v>-5.8599999999999997E-11</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="9">
         <v>-5.8599999999999997E-11</v>
       </c>
       <c r="J6" s="3">
@@ -1281,10 +1314,13 @@
       <c r="X6" s="3">
         <v>0</v>
       </c>
+      <c r="Y6" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9" t="s">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1353,10 +1389,13 @@
       <c r="X7" s="3">
         <v>130</v>
       </c>
+      <c r="Y7" s="3">
+        <v>330</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="1" t="s">
         <v>30</v>
       </c>
@@ -1423,10 +1462,13 @@
       <c r="X8" s="3">
         <v>0</v>
       </c>
+      <c r="Y8" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="1" t="s">
         <v>31</v>
       </c>
@@ -1493,10 +1535,13 @@
       <c r="X9" s="3">
         <v>0</v>
       </c>
+      <c r="Y9" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="1" t="s">
         <v>32</v>
       </c>
@@ -1563,10 +1608,13 @@
       <c r="X10" s="3">
         <v>0</v>
       </c>
+      <c r="Y10" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
@@ -1633,10 +1681,13 @@
       <c r="X11" s="3">
         <v>0</v>
       </c>
+      <c r="Y11" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8" t="s">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1706,10 +1757,13 @@
       <c r="X12" s="3">
         <v>700</v>
       </c>
+      <c r="Y12" s="3">
+        <v>1200</v>
+      </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="1" t="s">
         <v>36</v>
       </c>
@@ -1777,10 +1831,13 @@
       <c r="X13" s="3">
         <v>0</v>
       </c>
+      <c r="Y13" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="1" t="s">
         <v>37</v>
       </c>
@@ -1791,7 +1848,7 @@
       <c r="E14" s="3">
         <v>0</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="9">
         <v>-5.1500000000000001E-3</v>
       </c>
       <c r="G14" s="3">
@@ -1848,10 +1905,13 @@
       <c r="X14" s="3">
         <v>0</v>
       </c>
+      <c r="Y14" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="1" t="s">
         <v>38</v>
       </c>
@@ -1862,7 +1922,7 @@
       <c r="E15" s="3">
         <v>0</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="9">
         <v>1.5830000000000001E-7</v>
       </c>
       <c r="G15" s="3">
@@ -1919,10 +1979,13 @@
       <c r="X15" s="3">
         <v>0</v>
       </c>
+      <c r="Y15" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="1" t="s">
         <v>39</v>
       </c>
@@ -1989,12 +2052,15 @@
       <c r="X16" s="3">
         <v>0</v>
       </c>
+      <c r="Y16" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -2063,10 +2129,13 @@
       <c r="X17" s="3">
         <v>1</v>
       </c>
+      <c r="Y17" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="1" t="s">
         <v>41</v>
       </c>
@@ -2133,10 +2202,13 @@
       <c r="X18" s="3">
         <v>0</v>
       </c>
+      <c r="Y18" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="1" t="s">
         <v>42</v>
       </c>
@@ -2203,10 +2275,13 @@
       <c r="X19" s="3">
         <v>0</v>
       </c>
+      <c r="Y19" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="1" t="s">
         <v>43</v>
       </c>
@@ -2273,10 +2348,13 @@
       <c r="X20" s="3">
         <v>0</v>
       </c>
+      <c r="Y20" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="1" t="s">
         <v>44</v>
       </c>
@@ -2343,10 +2421,13 @@
       <c r="X21" s="3">
         <v>0</v>
       </c>
+      <c r="Y21" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="9" t="s">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -2415,10 +2496,13 @@
       <c r="X22" s="3">
         <v>1</v>
       </c>
+      <c r="Y22" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="1" t="s">
         <v>46</v>
       </c>
@@ -2486,10 +2570,13 @@
       <c r="X23" s="3">
         <v>0</v>
       </c>
+      <c r="Y23" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="1" t="s">
         <v>47</v>
       </c>
@@ -2556,10 +2643,13 @@
       <c r="X24" s="3">
         <v>0</v>
       </c>
+      <c r="Y24" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="1" t="s">
         <v>48</v>
       </c>
@@ -2626,10 +2716,13 @@
       <c r="X25" s="3">
         <v>0</v>
       </c>
+      <c r="Y25" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="1" t="s">
         <v>49</v>
       </c>
@@ -2696,10 +2789,13 @@
       <c r="X26" s="3">
         <v>0</v>
       </c>
+      <c r="Y26" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8" t="s">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -2768,10 +2864,13 @@
       <c r="X27" s="3">
         <v>1</v>
       </c>
+      <c r="Y27" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="1" t="s">
         <v>51</v>
       </c>
@@ -2838,10 +2937,13 @@
       <c r="X28" s="3">
         <v>0</v>
       </c>
+      <c r="Y28" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="1" t="s">
         <v>52</v>
       </c>
@@ -2908,10 +3010,13 @@
       <c r="X29" s="3">
         <v>0</v>
       </c>
+      <c r="Y29" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="1" t="s">
         <v>53</v>
       </c>
@@ -2978,10 +3083,13 @@
       <c r="X30" s="3">
         <v>0</v>
       </c>
+      <c r="Y30" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="1" t="s">
         <v>54</v>
       </c>
@@ -3048,8 +3156,11 @@
       <c r="X31" s="3">
         <v>0</v>
       </c>
+      <c r="Y31" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>55</v>
       </c>
@@ -3122,8 +3233,11 @@
       <c r="X32" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="Y32" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>58</v>
       </c>
@@ -3196,8 +3310,11 @@
       <c r="X33" s="3">
         <v>0</v>
       </c>
+      <c r="Y33" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>60</v>
       </c>
@@ -3270,8 +3387,11 @@
       <c r="X34" s="3">
         <v>0</v>
       </c>
+      <c r="Y34" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>63</v>
       </c>
@@ -3342,6 +3462,9 @@
         <v>0</v>
       </c>
       <c r="X35" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="13">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed any vestiges of proprietary information. In the future I want to have an opensource materials database of common things with references. Just need more than 0.1s per day to work on it
</commit_message>
<xml_diff>
--- a/Material_Properties.xlsx
+++ b/Material_Properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Transfer\Fraser Jones\1D_Transient_Toolbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B12C9B-76E5-4BC5-B3D5-792BAE9C2BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F635B348-03FE-4A02-95FE-455898CC5585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5FC984CA-FA47-49C6-B571-C8119F27FD36}"/>
   </bookViews>
@@ -402,13 +402,13 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -864,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{476E0231-AF0F-4564-A165-BC653E59D282}">
   <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,10 +950,10 @@
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1027,8 +1027,8 @@
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="1" t="s">
         <v>24</v>
       </c>
@@ -1100,8 +1100,8 @@
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
@@ -1173,8 +1173,8 @@
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
@@ -1246,8 +1246,8 @@
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="1" t="s">
         <v>27</v>
       </c>
@@ -1319,8 +1319,8 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1394,8 +1394,8 @@
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="1" t="s">
         <v>30</v>
       </c>
@@ -1467,8 +1467,8 @@
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="1" t="s">
         <v>31</v>
       </c>
@@ -1540,8 +1540,8 @@
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="1" t="s">
         <v>32</v>
       </c>
@@ -1613,8 +1613,8 @@
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
@@ -1686,8 +1686,8 @@
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11" t="s">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1762,8 +1762,8 @@
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="1" t="s">
         <v>36</v>
       </c>
@@ -1836,8 +1836,8 @@
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="1" t="s">
         <v>37</v>
       </c>
@@ -1910,8 +1910,8 @@
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="1" t="s">
         <v>38</v>
       </c>
@@ -1984,8 +1984,8 @@
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="1" t="s">
         <v>39</v>
       </c>
@@ -2057,10 +2057,10 @@
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="12" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -2073,7 +2073,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="3">
-        <v>1</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="G17" s="3">
         <v>1</v>
@@ -2134,8 +2134,8 @@
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="1" t="s">
         <v>41</v>
       </c>
@@ -2146,7 +2146,8 @@
         <v>0</v>
       </c>
       <c r="F18" s="3">
-        <v>0</v>
+        <f>1-F17</f>
+        <v>0.83299999999999996</v>
       </c>
       <c r="G18" s="3">
         <v>0</v>
@@ -2207,8 +2208,8 @@
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="1" t="s">
         <v>42</v>
       </c>
@@ -2280,8 +2281,8 @@
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="1" t="s">
         <v>43</v>
       </c>
@@ -2353,8 +2354,8 @@
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
       <c r="C21" s="1" t="s">
         <v>44</v>
       </c>
@@ -2426,8 +2427,8 @@
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="12" t="s">
+      <c r="A22" s="12"/>
+      <c r="B22" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -2440,7 +2441,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="3">
-        <v>0.16700000000000001</v>
+        <v>1</v>
       </c>
       <c r="G22" s="3">
         <v>1</v>
@@ -2501,8 +2502,8 @@
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
       <c r="C23" s="1" t="s">
         <v>46</v>
       </c>
@@ -2513,8 +2514,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="3">
-        <f>1-F22</f>
-        <v>0.83299999999999996</v>
+        <v>0</v>
       </c>
       <c r="G23" s="3">
         <v>0</v>
@@ -2575,8 +2575,8 @@
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="1" t="s">
         <v>47</v>
       </c>
@@ -2648,8 +2648,8 @@
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="1" t="s">
         <v>48</v>
       </c>
@@ -2721,8 +2721,8 @@
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
       <c r="C26" s="1" t="s">
         <v>49</v>
       </c>
@@ -2794,8 +2794,8 @@
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11" t="s">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -2869,8 +2869,8 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="1" t="s">
         <v>51</v>
       </c>
@@ -2942,8 +2942,8 @@
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="1" t="s">
         <v>52</v>
       </c>
@@ -3015,8 +3015,8 @@
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="1" t="s">
         <v>53</v>
       </c>
@@ -3088,8 +3088,8 @@
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="1" t="s">
         <v>54</v>
       </c>
@@ -3464,7 +3464,7 @@
       <c r="X35" s="3">
         <v>0</v>
       </c>
-      <c r="Y35" s="13">
+      <c r="Y35" s="11">
         <v>0</v>
       </c>
     </row>

</xml_diff>